<commit_message>
add Ethernet card to inventory
</commit_message>
<xml_diff>
--- a/Manufacturing/Equipment_Record.xlsx
+++ b/Manufacturing/Equipment_Record.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="30">
   <si>
     <t>Hardware Version</t>
   </si>
@@ -100,6 +100,15 @@
   </si>
   <si>
     <t>San Diego - Dixon</t>
+  </si>
+  <si>
+    <t>10G Ethernet card</t>
+  </si>
+  <si>
+    <t>10 GIGABIT ETHERNET PCIE ADAPTER CARD FOR DESKTOP - ETTUS RESEARCH</t>
+  </si>
+  <si>
+    <t>HC2494813</t>
   </si>
 </sst>
 </file>
@@ -494,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -845,6 +854,20 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Add ammo box for a test
The ammo box turned out to be too small to contain all the equipment
for the Palomar site, but we have it in inventory nonetheless.
</commit_message>
<xml_diff>
--- a/Manufacturing/Equipment_Record.xlsx
+++ b/Manufacturing/Equipment_Record.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="33">
   <si>
     <t>Hardware Version</t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>HC2494813</t>
+  </si>
+  <si>
+    <t>ammo box</t>
+  </si>
+  <si>
+    <t>from Harbor Freight</t>
+  </si>
+  <si>
+    <t>Golden Home</t>
   </si>
 </sst>
 </file>
@@ -503,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -868,6 +877,17 @@
         <v>15</v>
       </c>
     </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Added X310 USRP Kit
</commit_message>
<xml_diff>
--- a/Manufacturing/Equipment_Record.xlsx
+++ b/Manufacturing/Equipment_Record.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3280" yWindow="340" windowWidth="25600" windowHeight="14960" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="33">
   <si>
     <t>Hardware Version</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Item</t>
   </si>
   <si>
-    <t>USRP</t>
-  </si>
-  <si>
     <t>USRP B210 SDR KIT 2x2 (70MHz to 6GHz) with USB Cable</t>
   </si>
   <si>
@@ -109,6 +106,18 @@
   </si>
   <si>
     <t>HC2494813</t>
+  </si>
+  <si>
+    <t>USRP X310</t>
+  </si>
+  <si>
+    <t>USRP B210</t>
+  </si>
+  <si>
+    <t>USRP X310 KIT (KINTEX7-410T FPGA, 2 CHANNELS, 10GIGE AND PCIE BUS)</t>
+  </si>
+  <si>
+    <t>PA1289856</t>
   </si>
 </sst>
 </file>
@@ -503,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD24"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -545,207 +554,207 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -758,7 +767,7 @@
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -771,7 +780,7 @@
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -784,7 +793,7 @@
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -797,7 +806,7 @@
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -810,7 +819,7 @@
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -823,7 +832,7 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -836,7 +845,7 @@
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -849,23 +858,37 @@
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
         <v>27</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>28</v>
       </c>
-      <c r="C23" t="s">
+      <c r="E23" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>15</v>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected for RF daughter cards for X300
</commit_message>
<xml_diff>
--- a/Manufacturing/Equipment_Record.xlsx
+++ b/Manufacturing/Equipment_Record.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="21820" yWindow="6440" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="37">
   <si>
     <t>Hardware Version</t>
   </si>
@@ -118,6 +118,18 @@
   </si>
   <si>
     <t>PA1289856</t>
+  </si>
+  <si>
+    <t>UBX-40</t>
+  </si>
+  <si>
+    <t>UBX-40 USRP DAUGHTERBOARD (10 MHZ - 6 GHZ, 40 MHZ BW) - ETTUS RESEARCH</t>
+  </si>
+  <si>
+    <t>PA1288699</t>
+  </si>
+  <si>
+    <t>PA1288706</t>
   </si>
 </sst>
 </file>
@@ -512,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -891,6 +903,34 @@
         <v>14</v>
       </c>
     </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>